<commit_message>
elimine una clase que no servia
elimine una clase que no servia
</commit_message>
<xml_diff>
--- a/calendario.xlsx
+++ b/calendario.xlsx
@@ -936,27 +936,27 @@
       </c>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>31-Oct</t>
         </is>
       </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>29-Nov</t>
         </is>
       </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>4-Dic</t>
         </is>
       </c>
       <c r="F8" s="14" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>12-Dic</t>
         </is>
       </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>17-Dic</t>
         </is>
       </c>
       <c r="H8" s="3" t="n"/>
@@ -975,27 +975,32 @@
       </c>
       <c r="C9" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 30 de Octubre 
+ Aula C-101 - 7:00</t>
         </is>
       </c>
       <c r="D9" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 27 de Noviembre 
+ Aula C-101 - 7:00</t>
         </is>
       </c>
       <c r="E9" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 29 de Noviembre 
+ Aula C-101 - 7:00</t>
         </is>
       </c>
       <c r="F9" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Martes 10 de Diciembre 
+ Aula C-101 - 7:00</t>
         </is>
       </c>
       <c r="G9" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 13 de Diciembre 
+ Lab 5 - 12:40</t>
         </is>
       </c>
       <c r="H9" s="4" t="n"/>
@@ -1003,38 +1008,43 @@
     <row customHeight="1" ht="50.1" r="10">
       <c r="A10" s="13" t="inlineStr">
         <is>
-          <t>DESARROLLO DE HABILIDADES DEL PENSAMIENTO LÓGICO</t>
+          <t>METODOLOGÍA DE LA PROGRAMACIÓN</t>
         </is>
       </c>
       <c r="B10" s="21" t="inlineStr">
         <is>
-          <t>Martes 24 de Septiembre 
- Lab 4 - 9:00</t>
+          <t>Jueves 26 de Septiembre 
+ Lab 2 - 12:40</t>
         </is>
       </c>
       <c r="C10" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 25 de Octubre 
+ Lab 6 - 9:00</t>
         </is>
       </c>
       <c r="D10" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Jueves 28 de Noviembre 
+ Lab 2 - 12:40</t>
         </is>
       </c>
       <c r="E10" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Jueves 28 de Noviembre 
+ Lab 2 - 12:40</t>
         </is>
       </c>
       <c r="F10" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 11 de Diciembre 
+ Lab 6 - 9:50</t>
         </is>
       </c>
       <c r="G10" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 13 de Diciembre 
+ Lab 5 - 11:00</t>
         </is>
       </c>
       <c r="H10" s="4" t="n"/>
@@ -1042,38 +1052,43 @@
     <row customHeight="1" ht="50.1" r="11">
       <c r="A11" s="17" t="inlineStr">
         <is>
-          <t>METODOLOGÍA DE LA PROGRAMACIÓN</t>
+          <t>DESARROLLO DE HABILIDADES DEL PENSAMIENTO LÓGICO</t>
         </is>
       </c>
       <c r="B11" s="21" t="inlineStr">
         <is>
           <t>Viernes 27 de Septiembre 
- Lab 2 - 9:00</t>
+ Aula C-103 - 13:30</t>
         </is>
       </c>
       <c r="C11" s="22" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Martes 29 de Octubre 
+ Aula C-101 - 12:40</t>
         </is>
       </c>
       <c r="D11" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Martes 26 de Noviembre 
+ Aula C-101 - 12:40</t>
         </is>
       </c>
       <c r="E11" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Martes 3 de Diciembre 
+ Aula C-101 - 12:40</t>
         </is>
       </c>
       <c r="F11" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 11 de Diciembre 
+ Aula C-101 - 7:50</t>
         </is>
       </c>
       <c r="G11" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 13 de Diciembre 
+ Aula C-101 - 7:50</t>
         </is>
       </c>
       <c r="H11" s="4" t="n"/>
@@ -1092,27 +1107,32 @@
       </c>
       <c r="C12" s="20" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Lunes 28 de Octubre 
+ Aula C-101 - 7:00</t>
         </is>
       </c>
       <c r="D12" s="20" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Lunes 25 de Noviembre 
+ Aula C-101 - 7:00</t>
         </is>
       </c>
       <c r="E12" s="20" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Lunes 2 de Diciembre 
+ Aula C-101 - 7:00</t>
         </is>
       </c>
       <c r="F12" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 11 de Diciembre 
+ Lab 6 - 9:00</t>
         </is>
       </c>
       <c r="G12" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 13 de Diciembre 
+ Lab 6 - 9:50</t>
         </is>
       </c>
       <c r="H12" s="4" t="n"/>
@@ -1131,27 +1151,32 @@
       </c>
       <c r="C13" s="22" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Jueves 24 de Octubre 
+ Lab 2 - 9:00</t>
         </is>
       </c>
       <c r="D13" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 27 de Noviembre 
+ Lab 6 - 9:00</t>
         </is>
       </c>
       <c r="E13" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 27 de Noviembre 
+ Lab 6 - 9:00</t>
         </is>
       </c>
       <c r="F13" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 11 de Diciembre 
+ Lab1 - 11:00</t>
         </is>
       </c>
       <c r="G13" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 13 de Diciembre 
+ Lab 6 - 9:00</t>
         </is>
       </c>
       <c r="H13" s="4" t="n"/>
@@ -1170,27 +1195,32 @@
       </c>
       <c r="C14" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Lunes 28 de Octubre 
+ Aula C-101 - 11:00</t>
         </is>
       </c>
       <c r="D14" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Lunes 25 de Noviembre 
+ Aula C-101 - 11:00</t>
         </is>
       </c>
       <c r="E14" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Lunes 2 de Diciembre 
+ Aula C-101 - 11:00</t>
         </is>
       </c>
       <c r="F14" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 11 de Diciembre 
+ Aula C-101 - 7:00</t>
         </is>
       </c>
       <c r="G14" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 13 de Diciembre 
+ Aula C-101 - 7:00</t>
         </is>
       </c>
       <c r="H14" s="4" t="n"/>
@@ -1209,27 +1239,32 @@
       </c>
       <c r="C15" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 30 de Octubre 
+ Lab1 - 11:00</t>
         </is>
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 22 de Noviembre 
+ Lab 5 - 11:00</t>
         </is>
       </c>
       <c r="E15" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 29 de Noviembre 
+ Lab 5 - 11:00</t>
         </is>
       </c>
       <c r="F15" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Miercoles 11 de Diciembre 
+ Lab1 - 11:50</t>
         </is>
       </c>
       <c r="G15" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Viernes 13 de Diciembre 
+ Lab 5 - 11:50</t>
         </is>
       </c>
       <c r="H15" s="4" t="n"/>
@@ -1247,27 +1282,27 @@
       </c>
       <c r="C16" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>De acuerdo a la coordinación de inglés</t>
         </is>
       </c>
       <c r="D16" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>De acuerdo a la coordinación de inglés</t>
         </is>
       </c>
       <c r="E16" s="21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>De acuerdo a la coordinación de inglés</t>
         </is>
       </c>
       <c r="F16" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>De acuerdo a la coordinación de inglés</t>
         </is>
       </c>
       <c r="G16" s="16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>De acuerdo a la coordinación de inglés</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
bug cambio de diseño pagina
</commit_message>
<xml_diff>
--- a/calendario.xlsx
+++ b/calendario.xlsx
@@ -864,7 +864,7 @@
     <row r="2" ht="33.75" customHeight="1">
       <c r="B2" s="23" t="inlineStr">
         <is>
-          <t>1F-IRD</t>
+          <t>3A-DSM</t>
         </is>
       </c>
     </row>
@@ -931,32 +931,32 @@
       </c>
       <c r="B8" s="14" t="inlineStr">
         <is>
-          <t>4-Oct</t>
+          <t>2-Jun</t>
         </is>
       </c>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>31-Oct</t>
+          <t>24-Jun</t>
         </is>
       </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
-          <t>29-Nov</t>
+          <t>25-Jun</t>
         </is>
       </c>
       <c r="E8" s="14" t="inlineStr">
         <is>
-          <t>4-Dic</t>
+          <t>9-Jul</t>
         </is>
       </c>
       <c r="F8" s="14" t="inlineStr">
         <is>
-          <t>12-Dic</t>
+          <t>23-Jul</t>
         </is>
       </c>
       <c r="G8" s="14" t="inlineStr">
         <is>
-          <t>17-Dic</t>
+          <t>24-Jul</t>
         </is>
       </c>
       <c r="H8" s="3" t="n"/>
@@ -964,43 +964,43 @@
     <row r="9" ht="50.1" customHeight="1">
       <c r="A9" s="12" t="inlineStr">
         <is>
-          <t>FORMACIÓN SOCIOCULTURAL I</t>
+          <t>PROBABILIDAD Y ESTADÍSTICA</t>
         </is>
       </c>
       <c r="B9" s="21" t="inlineStr">
         <is>
-          <t>Jueves 26 de Septiembre 
- Aula C-104 - 9:00</t>
+          <t>Martes 26 de Mayo 
+ Aula C-20 - 7:00</t>
         </is>
       </c>
       <c r="C9" s="21" t="inlineStr">
         <is>
-          <t>Jueves 24 de Octubre 
- Aula C-104 - 9:00</t>
+          <t>Martes 23 de Junio 
+ Aula C-20 - 7:00</t>
         </is>
       </c>
       <c r="D9" s="21" t="inlineStr">
         <is>
-          <t>Jueves 28 de Noviembre 
- Aula C-104 - 9:00</t>
+          <t>Martes 23 de Junio 
+ Aula C-20 - 7:00</t>
         </is>
       </c>
       <c r="E9" s="21" t="inlineStr">
         <is>
-          <t>Jueves 28 de Noviembre 
- Aula C-104 - 9:00</t>
+          <t>Martes 7 de Julio 
+ Aula C-20 - 7:00</t>
         </is>
       </c>
       <c r="F9" s="16" t="inlineStr">
         <is>
-          <t>Miercoles 11 de Diciembre 
- Lab 4 - 7:00</t>
+          <t>Miercoles 22 de Julio 
+ Lab4 - 11:00</t>
         </is>
       </c>
       <c r="G9" s="16" t="inlineStr">
         <is>
-          <t>Viernes 13 de Diciembre 
- Aula C-104 - 7:50</t>
+          <t>Jueves 23 de Julio 
+ Aula C-17 - 12:40</t>
         </is>
       </c>
       <c r="H9" s="4" t="n"/>
@@ -1008,43 +1008,43 @@
     <row r="10" ht="50.1" customHeight="1">
       <c r="A10" s="13" t="inlineStr">
         <is>
-          <t>METODOLOGÍA DE LA PROGRAMACIÓN</t>
+          <t>FORMACIÓN SOCIOCULTURAL III</t>
         </is>
       </c>
       <c r="B10" s="21" t="inlineStr">
         <is>
-          <t>Viernes 27 de Septiembre 
- Lab 9 - 11:00</t>
+          <t>Jueves 28 de Mayo 
+ Aula C-16 - 7:00</t>
         </is>
       </c>
       <c r="C10" s="21" t="inlineStr">
         <is>
-          <t>Viernes 25 de Octubre 
- Lab 9 - 11:00</t>
+          <t>Jueves 18 de Junio 
+ Aula C-16 - 7:00</t>
         </is>
       </c>
       <c r="D10" s="21" t="inlineStr">
         <is>
-          <t>Viernes 22 de Noviembre 
- Lab 9 - 11:00</t>
+          <t>Jueves 18 de Junio 
+ Aula C-16 - 7:00</t>
         </is>
       </c>
       <c r="E10" s="21" t="inlineStr">
         <is>
-          <t>Viernes 29 de Noviembre 
- Lab 9 - 11:00</t>
+          <t>Jueves 2 de Julio 
+ Aula C-16 - 7:00</t>
         </is>
       </c>
       <c r="F10" s="16" t="inlineStr">
         <is>
-          <t>Miercoles 11 de Diciembre 
- Aula C-104 - 9:50</t>
+          <t>Miercoles 22 de Julio 
+ Aula C-23 - 7:00</t>
         </is>
       </c>
       <c r="G10" s="16" t="inlineStr">
         <is>
-          <t>Viernes 13 de Diciembre 
- Lab 9 - 11:50</t>
+          <t>Jueves 23 de Julio 
+ Aula C-16 - 7:00</t>
         </is>
       </c>
       <c r="H10" s="4" t="n"/>
@@ -1052,43 +1052,43 @@
     <row r="11" ht="50.1" customHeight="1">
       <c r="A11" s="17" t="inlineStr">
         <is>
-          <t>EXPRESIÓN ORAL Y ESCRITA I</t>
+          <t>CALCULO DIFERENCIAL</t>
         </is>
       </c>
       <c r="B11" s="21" t="inlineStr">
         <is>
-          <t>Lunes 30 de Septiembre 
- Aula C-104 - 7:00</t>
+          <t>Viernes 29 de Mayo 
+ Aula C-17 - 7:00</t>
         </is>
       </c>
       <c r="C11" s="22" t="inlineStr">
         <is>
-          <t>Miercoles 30 de Octubre 
- Aula C-104 - 9:00</t>
+          <t>Viernes 19 de Junio 
+ Aula C-17 - 7:00</t>
         </is>
       </c>
       <c r="D11" s="21" t="inlineStr">
         <is>
-          <t>Lunes 25 de Noviembre 
- Aula C-104 - 7:00</t>
+          <t>Viernes 19 de Junio 
+ Aula C-17 - 7:00</t>
         </is>
       </c>
       <c r="E11" s="21" t="inlineStr">
         <is>
-          <t>Miercoles 27 de Noviembre 
- Aula C-104 - 9:00</t>
+          <t>Viernes 3 de Julio 
+ Aula C-17 - 7:00</t>
         </is>
       </c>
       <c r="F11" s="16" t="inlineStr">
         <is>
-          <t>Miercoles 11 de Diciembre 
- Aula C-104 - 9:00</t>
+          <t>Miercoles 22 de Julio 
+ Lab8 - 9:00</t>
         </is>
       </c>
       <c r="G11" s="16" t="inlineStr">
         <is>
-          <t>Viernes 13 de Diciembre 
- Lab 9 - 9:00</t>
+          <t>Jueves 23 de Julio 
+ Lab6 - 9:00</t>
         </is>
       </c>
       <c r="H11" s="4" t="n"/>
@@ -1096,43 +1096,43 @@
     <row r="12" ht="50.1" customHeight="1">
       <c r="A12" s="13" t="inlineStr">
         <is>
-          <t>FUNDAMENTOS DE REDES</t>
+          <t>APLICACIONES WEB</t>
         </is>
       </c>
       <c r="B12" s="20" t="inlineStr">
         <is>
-          <t>Miercoles 2 de Octubre 
- Lab 4 - 7:00</t>
+          <t>Miercoles 27 de Mayo 
+ Lab4 - 11:00</t>
         </is>
       </c>
       <c r="C12" s="20" t="inlineStr">
         <is>
-          <t>Martes 29 de Octubre 
- Aula C-103 - 9:00</t>
+          <t>Miercoles 17 de Junio 
+ Lab4 - 11:00</t>
         </is>
       </c>
       <c r="D12" s="20" t="inlineStr">
         <is>
-          <t>Miercoles 27 de Noviembre 
- Lab 4 - 7:00</t>
+          <t>Miercoles 24 de Junio 
+ Lab4 - 11:00</t>
         </is>
       </c>
       <c r="E12" s="20" t="inlineStr">
         <is>
-          <t>Martes 3 de Diciembre 
- Aula C-103 - 9:00</t>
+          <t>Miercoles 8 de Julio 
+ Lab4 - 11:00</t>
         </is>
       </c>
       <c r="F12" s="16" t="inlineStr">
         <is>
-          <t>Miercoles 11 de Diciembre 
- Aula C-104 - 11:50</t>
+          <t>Martes 21 de Julio 
+ Aula C-20 - 7:00</t>
         </is>
       </c>
       <c r="G12" s="16" t="inlineStr">
         <is>
-          <t>Viernes 13 de Diciembre 
- Lab 9 - 11:00</t>
+          <t>Miercoles 22 de Julio 
+ Aula C-23 - 7:00</t>
         </is>
       </c>
       <c r="H12" s="4" t="n"/>
@@ -1140,43 +1140,43 @@
     <row r="13" ht="50.1" customHeight="1">
       <c r="A13" s="12" t="inlineStr">
         <is>
-          <t>FUNDAMENTOS DE TI</t>
+          <t>INTEGRADORA I</t>
         </is>
       </c>
       <c r="B13" s="21" t="inlineStr">
         <is>
-          <t>Jueves 3 de Octubre 
- Lab 6 - 7:00</t>
+          <t>Viernes 29 de Mayo 
+ Lab3 - 11:00</t>
         </is>
       </c>
       <c r="C13" s="22" t="inlineStr">
         <is>
-          <t>Martes 29 de Octubre 
- Lab Elect - 7:00</t>
+          <t>Viernes 19 de Junio 
+ Lab3 - 11:00</t>
         </is>
       </c>
       <c r="D13" s="21" t="inlineStr">
         <is>
-          <t>Martes 26 de Noviembre 
- Lab Elect - 7:00</t>
+          <t>Viernes 19 de Junio 
+ Lab3 - 11:00</t>
         </is>
       </c>
       <c r="E13" s="21" t="inlineStr">
         <is>
-          <t>Martes 3 de Diciembre 
- Lab Elect - 7:00</t>
+          <t>Viernes 3 de Julio 
+ Lab3 - 11:00</t>
         </is>
       </c>
       <c r="F13" s="16" t="inlineStr">
         <is>
-          <t>Miercoles 11 de Diciembre 
- Aula C-104 - 11:00</t>
+          <t>Miercoles 22 de Julio 
+ Aula C-23 - 7:50</t>
         </is>
       </c>
       <c r="G13" s="16" t="inlineStr">
         <is>
-          <t>Viernes 13 de Diciembre 
- Lab 9 - 9:50</t>
+          <t>Jueves 23 de Julio 
+ Aula C-16 - 7:50</t>
         </is>
       </c>
       <c r="H13" s="4" t="n"/>
@@ -1184,43 +1184,43 @@
     <row r="14" ht="50.1" customHeight="1">
       <c r="A14" s="15" t="inlineStr">
         <is>
-          <t>ÁLGEBRA LINEAL</t>
+          <t>SISTEMAS OPERATIVOS</t>
         </is>
       </c>
       <c r="B14" s="21" t="inlineStr">
         <is>
-          <t>Lunes 30 de Septiembre 
- Aula C-104 - 9:00</t>
+          <t>Lunes 1 de Junio 
+ Lab8 - 9:00</t>
         </is>
       </c>
       <c r="C14" s="21" t="inlineStr">
         <is>
-          <t>Lunes 28 de Octubre 
- Aula C-104 - 9:00</t>
+          <t>Miercoles 17 de Junio 
+ Lab8 - 9:00</t>
         </is>
       </c>
       <c r="D14" s="21" t="inlineStr">
         <is>
-          <t>Lunes 25 de Noviembre 
- Aula C-104 - 9:00</t>
+          <t>Lunes 22 de Junio 
+ Lab8 - 9:00</t>
         </is>
       </c>
       <c r="E14" s="21" t="inlineStr">
         <is>
-          <t>Lunes 2 de Diciembre 
- Aula C-104 - 9:00</t>
+          <t>Lunes 6 de Julio 
+ Lab8 - 9:00</t>
         </is>
       </c>
       <c r="F14" s="16" t="inlineStr">
         <is>
-          <t>Martes 10 de Diciembre 
- Lab Elect - 7:00</t>
+          <t>Miercoles 22 de Julio 
+ Lab8 - 9:50</t>
         </is>
       </c>
       <c r="G14" s="16" t="inlineStr">
         <is>
-          <t>Viernes 13 de Diciembre 
- Aula C-104 - 12:40</t>
+          <t>Jueves 23 de Julio 
+ Lab6 - 9:50</t>
         </is>
       </c>
       <c r="H14" s="4" t="n"/>
@@ -1228,43 +1228,43 @@
     <row r="15" ht="50.1" customHeight="1">
       <c r="A15" s="12" t="inlineStr">
         <is>
-          <t>DESARROLLO DE HABILIDADES DEL PENSAMIENTO LÓGICO</t>
+          <t>BASES DE DATOS PARA APLICACIONES</t>
         </is>
       </c>
       <c r="B15" s="16" t="inlineStr">
         <is>
-          <t>Jueves 3 de Octubre 
- Aula C-104 - 12:40</t>
+          <t>Lunes 1 de Junio 
+ Lab2 - 11:00</t>
         </is>
       </c>
       <c r="C15" s="16" t="inlineStr">
         <is>
-          <t>Jueves 24 de Octubre 
- Aula C-104 - 12:40</t>
+          <t>Lunes 22 de Junio 
+ Lab2 - 11:00</t>
         </is>
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>Jueves 28 de Noviembre 
- Aula C-104 - 12:40</t>
+          <t>Lunes 22 de Junio 
+ Lab2 - 11:00</t>
         </is>
       </c>
       <c r="E15" s="16" t="inlineStr">
         <is>
-          <t>Jueves 28 de Noviembre 
- Aula C-104 - 12:40</t>
+          <t>Lunes 6 de Julio 
+ Lab2 - 11:00</t>
         </is>
       </c>
       <c r="F15" s="16" t="inlineStr">
         <is>
-          <t>Miercoles 11 de Diciembre 
- Lab 4 - 7:50</t>
+          <t>Miercoles 22 de Julio 
+ Lab4 - 11:50</t>
         </is>
       </c>
       <c r="G15" s="16" t="inlineStr">
         <is>
-          <t>Viernes 13 de Diciembre 
- Aula C-104 - 7:00</t>
+          <t>Jueves 23 de Julio 
+ Lab2 - 13:30</t>
         </is>
       </c>
       <c r="H15" s="4" t="n"/>
@@ -1272,7 +1272,7 @@
     <row r="16" ht="48" customHeight="1">
       <c r="A16" s="15" t="inlineStr">
         <is>
-          <t>INGLÉS I</t>
+          <t>INGLÉS III</t>
         </is>
       </c>
       <c r="B16" s="21" t="inlineStr">

</xml_diff>